<commit_message>
small fix to xlsx
</commit_message>
<xml_diff>
--- a/Notes/initial_BLEUandPINC.xlsx
+++ b/Notes/initial_BLEUandPINC.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22221"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2760" yWindow="240" windowWidth="24640" windowHeight="15560" tabRatio="500"/>
+    <workbookView xWindow="6580" yWindow="200" windowWidth="24640" windowHeight="15620" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
   <si>
     <t>16and7plays_16LM.1</t>
   </si>
@@ -88,6 +88,9 @@
   </si>
   <si>
     <t>phrase2.2</t>
+  </si>
+  <si>
+    <t>16plays_36LM_mert.2</t>
   </si>
 </sst>
 </file>
@@ -718,7 +721,6 @@
           <c:smooth val="0"/>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="r"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -726,11 +728,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="387812008"/>
-        <c:axId val="446249384"/>
+        <c:axId val="547861352"/>
+        <c:axId val="422253784"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="387812008"/>
+        <c:axId val="547861352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -759,12 +761,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="446249384"/>
+        <c:crossAx val="422253784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="446249384"/>
+        <c:axId val="422253784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="19.0"/>
@@ -795,7 +797,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="387812008"/>
+        <c:crossAx val="547861352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1176,8 +1178,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1311,13 +1313,13 @@
         <v>23.23</v>
       </c>
       <c r="D7">
-        <v>19.260000000000002</v>
+        <v>15.69</v>
       </c>
       <c r="E7">
-        <v>54.44</v>
+        <v>52.94</v>
       </c>
       <c r="F7" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:6">

</xml_diff>